<commit_message>
Refactor Source Code for paper.
</commit_message>
<xml_diff>
--- a/src/theorem/conclusions.xlsx
+++ b/src/theorem/conclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>constraint</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,10 @@
   </si>
   <si>
     <t>Behave better on bad conditions, no reason to cooperate.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1 &lt;= p2,p3 &lt;= p2,p3 &lt;= p4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -475,6 +479,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>